<commit_message>
Add stl and dxf files
</commit_message>
<xml_diff>
--- a/CAD/3d_print.xlsx
+++ b/CAD/3d_print.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\CAD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A86D27A-7A53-4525-816E-574208DF782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>motor_holder.STL</t>
+  </si>
+  <si>
+    <t>bearing_block.STL</t>
+  </si>
+  <si>
+    <t>wheel_mount.STL</t>
+  </si>
+  <si>
+    <t>3_in_stand_offs.STL</t>
+  </si>
+  <si>
+    <t>battery_holder.STL</t>
+  </si>
+  <si>
+    <t>jetson_orin_nano_holder.STL</t>
+  </si>
+  <si>
+    <t>9_inch_spacers_3prong.STL</t>
+  </si>
+  <si>
+    <t>astra_holder.STL</t>
+  </si>
+  <si>
+    <t>3.5_inch_cir_standoff.STL</t>
+  </si>
+  <si>
+    <t>bottom_support_left.STL</t>
+  </si>
+  <si>
+    <t>bottom_support_right.STL</t>
+  </si>
+  <si>
+    <t>top_support_left.STL</t>
+  </si>
+  <si>
+    <t>top_support_right.STL</t>
+  </si>
+  <si>
+    <t>microphone_casing_back.STL</t>
+  </si>
+  <si>
+    <t>microphone_casing.STL</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +401,147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="23.9453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update STLs for 7 mm board thickness and 80 mm wheel
</commit_message>
<xml_diff>
--- a/CAD/3d_print.xlsx
+++ b/CAD/3d_print.xlsx
@@ -1,65 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satom\Desktop\Robot\CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A86D27A-7A53-4525-816E-574208DF782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9C376F-5299-48B4-B498-BDDD7B4C3628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7530" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>File Name</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>motor_holder.STL</t>
   </si>
   <si>
-    <t>bearing_block.STL</t>
-  </si>
-  <si>
     <t>wheel_mount.STL</t>
   </si>
   <si>
     <t>3_in_stand_offs.STL</t>
   </si>
   <si>
-    <t>battery_holder.STL</t>
-  </si>
-  <si>
-    <t>jetson_orin_nano_holder.STL</t>
-  </si>
-  <si>
-    <t>9_inch_spacers_3prong.STL</t>
-  </si>
-  <si>
     <t>astra_holder.STL</t>
   </si>
   <si>
-    <t>3.5_inch_cir_standoff.STL</t>
-  </si>
-  <si>
     <t>bottom_support_left.STL</t>
   </si>
   <si>
@@ -76,6 +69,45 @@
   </si>
   <si>
     <t>microphone_casing.STL</t>
+  </si>
+  <si>
+    <t>wheel_bearing_block.STL</t>
+  </si>
+  <si>
+    <t>Quantity/Robot</t>
+  </si>
+  <si>
+    <t>Quantity (Total)</t>
+  </si>
+  <si>
+    <t>NiMH_Holder_Front.STL</t>
+  </si>
+  <si>
+    <t>NiMH_Holder_Back.STL</t>
+  </si>
+  <si>
+    <t>jetson_orin_nano_holder_corner_1</t>
+  </si>
+  <si>
+    <t>jetson_orin_nano_holder_corner_2</t>
+  </si>
+  <si>
+    <t>9_inch_spacer.STL</t>
+  </si>
+  <si>
+    <t>3.5_inch_standoff.STL</t>
+  </si>
+  <si>
+    <t>Estimated Filament/robot (g)</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Number of Robots:</t>
+  </si>
+  <si>
+    <t>Filament (g, Total)</t>
   </si>
 </sst>
 </file>
@@ -99,12 +131,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,9 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,146 +444,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="23.9453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.20703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.05078125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C4">
+        <f>B4*10.78</f>
+        <v>21.56</v>
+      </c>
+      <c r="D4">
+        <f>B4*$B$1</f>
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <f>C4*$B$1</f>
+        <v>86.24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>B5*6.15</f>
+        <v>24.6</v>
+      </c>
+      <c r="D5">
+        <f>B5*$B$1</f>
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f>C5*$B$1</f>
+        <v>98.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f>B6*1.95</f>
+        <v>7.8</v>
+      </c>
+      <c r="D6">
+        <f>B6*$B$1</f>
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <f>C6*$B$1</f>
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+      <c r="B7">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
+      <c r="C7">
+        <f>4.4*B7</f>
+        <v>35.200000000000003</v>
+      </c>
+      <c r="D7">
+        <f>B7*$B$1</f>
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <f>C7*$B$1</f>
+        <v>140.80000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="C8">
+        <f>B8*12.01</f>
+        <v>24.02</v>
+      </c>
+      <c r="D8">
+        <f>B8*$B$1</f>
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="E8">
+        <f>C8*$B$1</f>
+        <v>96.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <f>B9*12.39</f>
+        <v>24.78</v>
+      </c>
+      <c r="D9">
+        <f>B9*$B$1</f>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <f>C9*$B$1</f>
+        <v>99.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f>B10*3.25</f>
+        <v>6.5</v>
+      </c>
+      <c r="D10">
+        <f>B10*$B$1</f>
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f>C10*$B$1</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <f>B11*3.25</f>
+        <v>6.5</v>
+      </c>
+      <c r="D11">
+        <f>B11*$B$1</f>
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <f>C11*$B$1</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12">
+        <f>B12*29.28</f>
+        <v>351.36</v>
+      </c>
+      <c r="D12">
+        <f>B12*$B$1</f>
+        <v>48</v>
+      </c>
+      <c r="E12">
+        <f>C12*$B$1</f>
+        <v>1405.44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13">
+        <v>25.12</v>
+      </c>
+      <c r="D13">
+        <f>B13*$B$1</f>
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f>C13*$B$1</f>
+        <v>100.48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <f>B14*4.96</f>
+        <v>19.84</v>
+      </c>
+      <c r="D14">
+        <f>B14*$B$1</f>
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <f>C14*$B$1</f>
+        <v>79.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
+      <c r="C15">
+        <v>1.7</v>
+      </c>
+      <c r="D15">
+        <f>B15*$B$1</f>
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <f>C15*$B$1</f>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1.7</v>
+      </c>
+      <c r="D16">
+        <f>B16*$B$1</f>
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f>C16*$B$1</f>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>6.27</v>
+      </c>
+      <c r="D17">
+        <f>B17*$B$1</f>
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <f>C17*$B$1</f>
+        <v>25.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>6.27</v>
+      </c>
+      <c r="D18">
+        <f>B18*$B$1</f>
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <f>C18*$B$1</f>
+        <v>25.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
+      <c r="C19">
+        <f>B19*2.71</f>
+        <v>5.42</v>
+      </c>
+      <c r="D19">
+        <f>B19*$B$1</f>
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <f>C19*$B$1</f>
+        <v>21.68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
         <v>2</v>
+      </c>
+      <c r="C20">
+        <f>B20*1.42</f>
+        <v>2.84</v>
+      </c>
+      <c r="D20">
+        <f>B20*$B$1</f>
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <f>C20*$B$1</f>
+        <v>11.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
+        <f>SUM(C4:C20)</f>
+        <v>571.48</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2">
+        <f>SUM(E4:E20)</f>
+        <v>2285.92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>